<commit_message>
inicio de reporte pdf consolidado
</commit_message>
<xml_diff>
--- a/presupuesto/presupuesto_2020.xlsx
+++ b/presupuesto/presupuesto_2020.xlsx
@@ -406,16 +406,16 @@
         <v>montoCompMes</v>
       </c>
       <c r="I1" t="str">
+        <v>montoCompAcm</v>
+      </c>
+      <c r="J1" t="str">
         <v>montoCausMes</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
+        <v>montoCausAcm</v>
+      </c>
+      <c r="L1" t="str">
         <v>montoPagaMes</v>
-      </c>
-      <c r="K1" t="str">
-        <v>montoCompAcm</v>
-      </c>
-      <c r="L1" t="str">
-        <v>montoCausAcm</v>
       </c>
       <c r="M1" t="str">
         <v>montoPagaAcm</v>
@@ -426,13 +426,40 @@
         <v>04.00.00.00.000</v>
       </c>
       <c r="B2" t="str">
-        <v>00.00.00.00.000</v>
+        <v>04.00.00.00.000</v>
       </c>
       <c r="C2" t="str">
-        <v>&lt;&lt; CUENTA FALTANTE &gt;&gt;</v>
+        <v>GASTOS</v>
       </c>
       <c r="D2">
-        <v>1084247200</v>
+        <v>4541728600</v>
+      </c>
+      <c r="E2">
+        <v>723252261.3299999</v>
+      </c>
+      <c r="F2">
+        <v>2979395507.75</v>
+      </c>
+      <c r="G2">
+        <v>7521124107.75</v>
+      </c>
+      <c r="H2">
+        <v>1847270214.52</v>
+      </c>
+      <c r="I2">
+        <v>4064356250.46</v>
+      </c>
+      <c r="J2">
+        <v>1844363714.5</v>
+      </c>
+      <c r="K2">
+        <v>4071499472.8599997</v>
+      </c>
+      <c r="L2">
+        <v>1847116813.52</v>
+      </c>
+      <c r="M2">
+        <v>4057867127.06</v>
       </c>
     </row>
     <row r="3">
@@ -461,16 +488,16 @@
         <v>1117598567.21</v>
       </c>
       <c r="I3">
+        <v>2552263286.7599998</v>
+      </c>
+      <c r="J3">
         <v>1117598567.21</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>2549867036.7599998</v>
+      </c>
+      <c r="L3">
         <v>1116945166.21</v>
-      </c>
-      <c r="K3">
-        <v>2552263286.7599998</v>
-      </c>
-      <c r="L3">
-        <v>2549867036.7599998</v>
       </c>
       <c r="M3">
         <v>2554813635.7599998</v>
@@ -502,16 +529,16 @@
         <v>85358101.53</v>
       </c>
       <c r="I4">
-        <v>85358101.53</v>
+        <v>420091234.51</v>
       </c>
       <c r="J4">
         <v>85358101.53</v>
       </c>
       <c r="K4">
-        <v>420091234.51</v>
+        <v>417694984.51</v>
       </c>
       <c r="L4">
-        <v>417694984.51</v>
+        <v>85358101.53</v>
       </c>
       <c r="M4">
         <v>417694984.51</v>
@@ -543,7 +570,7 @@
         <v>52748101.53</v>
       </c>
       <c r="I5">
-        <v>52748101.53</v>
+        <v>252388943.19000003</v>
       </c>
       <c r="J5">
         <v>52748101.53</v>
@@ -552,7 +579,7 @@
         <v>252388943.19000003</v>
       </c>
       <c r="L5">
-        <v>252388943.19000003</v>
+        <v>52748101.53</v>
       </c>
       <c r="M5">
         <v>252388943.19000003</v>
@@ -584,7 +611,7 @@
         <v>9606000</v>
       </c>
       <c r="I6">
-        <v>9606000</v>
+        <v>46777671.55</v>
       </c>
       <c r="J6">
         <v>9606000</v>
@@ -593,7 +620,7 @@
         <v>46777671.55</v>
       </c>
       <c r="L6">
-        <v>46777671.55</v>
+        <v>9606000</v>
       </c>
       <c r="M6">
         <v>46777671.55</v>
@@ -625,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>5556558.62</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -634,7 +661,7 @@
         <v>5556558.62</v>
       </c>
       <c r="L7">
-        <v>5556558.62</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>5556558.62</v>
@@ -666,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>5556558.62</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -675,7 +702,7 @@
         <v>5556558.62</v>
       </c>
       <c r="L8">
-        <v>5556558.62</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>5556558.62</v>
@@ -748,16 +775,16 @@
         <v>23004000</v>
       </c>
       <c r="I10">
-        <v>23004000</v>
+        <v>115368061.15</v>
       </c>
       <c r="J10">
         <v>23004000</v>
       </c>
       <c r="K10">
-        <v>115368061.15</v>
+        <v>112971811.15</v>
       </c>
       <c r="L10">
-        <v>112971811.15</v>
+        <v>23004000</v>
       </c>
       <c r="M10">
         <v>112971811.15</v>
@@ -789,16 +816,16 @@
         <v>45631808.36</v>
       </c>
       <c r="I11">
+        <v>213286058.21999997</v>
+      </c>
+      <c r="J11">
         <v>45631808.36</v>
-      </c>
-      <c r="J11">
-        <v>44978408.36</v>
       </c>
       <c r="K11">
         <v>213286058.21999997</v>
       </c>
       <c r="L11">
-        <v>213286058.21999997</v>
+        <v>44978408.36</v>
       </c>
       <c r="M11">
         <v>212632658.21999997</v>
@@ -830,7 +857,7 @@
         <v>12043948.32</v>
       </c>
       <c r="I12">
-        <v>12043948.32</v>
+        <v>55695842.12999998</v>
       </c>
       <c r="J12">
         <v>12043948.32</v>
@@ -839,7 +866,7 @@
         <v>55695842.12999998</v>
       </c>
       <c r="L12">
-        <v>55695842.12999998</v>
+        <v>12043948.32</v>
       </c>
       <c r="M12">
         <v>55695842.12999998</v>
@@ -871,7 +898,7 @@
         <v>14283268.04</v>
       </c>
       <c r="I13">
-        <v>14283268.04</v>
+        <v>66533129.629999995</v>
       </c>
       <c r="J13">
         <v>14283268.04</v>
@@ -880,7 +907,7 @@
         <v>66533129.629999995</v>
       </c>
       <c r="L13">
-        <v>66533129.629999995</v>
+        <v>14283268.04</v>
       </c>
       <c r="M13">
         <v>66533129.629999995</v>
@@ -912,16 +939,16 @@
         <v>1306800</v>
       </c>
       <c r="I14">
+        <v>6208984.2</v>
+      </c>
+      <c r="J14">
         <v>1306800</v>
-      </c>
-      <c r="J14">
-        <v>653400</v>
       </c>
       <c r="K14">
         <v>6208984.2</v>
       </c>
       <c r="L14">
-        <v>6208984.2</v>
+        <v>653400</v>
       </c>
       <c r="M14">
         <v>5555584.2</v>
@@ -953,7 +980,7 @@
         <v>300000</v>
       </c>
       <c r="I15">
-        <v>300000</v>
+        <v>1325000</v>
       </c>
       <c r="J15">
         <v>300000</v>
@@ -962,7 +989,7 @@
         <v>1325000</v>
       </c>
       <c r="L15">
-        <v>1325000</v>
+        <v>300000</v>
       </c>
       <c r="M15">
         <v>1325000</v>
@@ -1035,7 +1062,7 @@
         <v>6917280</v>
       </c>
       <c r="I17">
-        <v>6917280</v>
+        <v>30551320</v>
       </c>
       <c r="J17">
         <v>6917280</v>
@@ -1044,7 +1071,7 @@
         <v>30551320</v>
       </c>
       <c r="L17">
-        <v>30551320</v>
+        <v>6917280</v>
       </c>
       <c r="M17">
         <v>30551320</v>
@@ -1076,7 +1103,7 @@
         <v>6880512</v>
       </c>
       <c r="I18">
-        <v>6880512</v>
+        <v>34659282.26</v>
       </c>
       <c r="J18">
         <v>6880512</v>
@@ -1085,7 +1112,7 @@
         <v>34659282.26</v>
       </c>
       <c r="L18">
-        <v>34659282.26</v>
+        <v>6880512</v>
       </c>
       <c r="M18">
         <v>34659282.26</v>
@@ -1117,7 +1144,7 @@
         <v>3000000</v>
       </c>
       <c r="I19">
-        <v>3000000</v>
+        <v>14000000</v>
       </c>
       <c r="J19">
         <v>3000000</v>
@@ -1126,7 +1153,7 @@
         <v>14000000</v>
       </c>
       <c r="L19">
-        <v>14000000</v>
+        <v>3000000</v>
       </c>
       <c r="M19">
         <v>14000000</v>
@@ -1158,7 +1185,7 @@
         <v>900000</v>
       </c>
       <c r="I20">
-        <v>900000</v>
+        <v>4312500</v>
       </c>
       <c r="J20">
         <v>900000</v>
@@ -1167,7 +1194,7 @@
         <v>4312500</v>
       </c>
       <c r="L20">
-        <v>4312500</v>
+        <v>900000</v>
       </c>
       <c r="M20">
         <v>4312500</v>
@@ -1199,7 +1226,7 @@
         <v>76198400</v>
       </c>
       <c r="I21">
-        <v>76198400</v>
+        <v>303073816.56</v>
       </c>
       <c r="J21">
         <v>76198400</v>
@@ -1208,7 +1235,7 @@
         <v>303073816.56</v>
       </c>
       <c r="L21">
-        <v>303073816.56</v>
+        <v>76198400</v>
       </c>
       <c r="M21">
         <v>308673816.56</v>
@@ -1240,7 +1267,7 @@
         <v>18000000</v>
       </c>
       <c r="I22">
-        <v>18000000</v>
+        <v>82600000</v>
       </c>
       <c r="J22">
         <v>18000000</v>
@@ -1249,7 +1276,7 @@
         <v>82600000</v>
       </c>
       <c r="L22">
-        <v>82600000</v>
+        <v>18000000</v>
       </c>
       <c r="M22">
         <v>88200000</v>
@@ -1281,7 +1308,7 @@
         <v>6000000</v>
       </c>
       <c r="I23">
-        <v>6000000</v>
+        <v>28000000</v>
       </c>
       <c r="J23">
         <v>6000000</v>
@@ -1290,7 +1317,7 @@
         <v>28000000</v>
       </c>
       <c r="L23">
-        <v>28000000</v>
+        <v>6000000</v>
       </c>
       <c r="M23">
         <v>28000000</v>
@@ -1322,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>800000</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1331,7 +1358,7 @@
         <v>800000</v>
       </c>
       <c r="L24">
-        <v>800000</v>
+        <v>0</v>
       </c>
       <c r="M24">
         <v>800000</v>
@@ -1363,7 +1390,7 @@
         <v>4800000</v>
       </c>
       <c r="I25">
-        <v>4800000</v>
+        <v>22400000</v>
       </c>
       <c r="J25">
         <v>4800000</v>
@@ -1372,7 +1399,7 @@
         <v>22400000</v>
       </c>
       <c r="L25">
-        <v>22400000</v>
+        <v>4800000</v>
       </c>
       <c r="M25">
         <v>22400000</v>
@@ -1404,7 +1431,7 @@
         <v>12268800</v>
       </c>
       <c r="I26">
-        <v>12268800</v>
+        <v>44101955.66</v>
       </c>
       <c r="J26">
         <v>12268800</v>
@@ -1413,7 +1440,7 @@
         <v>44101955.66</v>
       </c>
       <c r="L26">
-        <v>44101955.66</v>
+        <v>12268800</v>
       </c>
       <c r="M26">
         <v>44101955.66</v>
@@ -1445,7 +1472,7 @@
         <v>30006400</v>
       </c>
       <c r="I27">
-        <v>30006400</v>
+        <v>105844394.65</v>
       </c>
       <c r="J27">
         <v>30006400</v>
@@ -1454,7 +1481,7 @@
         <v>105844394.65</v>
       </c>
       <c r="L27">
-        <v>105844394.65</v>
+        <v>30006400</v>
       </c>
       <c r="M27">
         <v>105844394.65</v>
@@ -1486,7 +1513,7 @@
         <v>5123200</v>
       </c>
       <c r="I28">
-        <v>5123200</v>
+        <v>19327466.25</v>
       </c>
       <c r="J28">
         <v>5123200</v>
@@ -1495,7 +1522,7 @@
         <v>19327466.25</v>
       </c>
       <c r="L28">
-        <v>19327466.25</v>
+        <v>5123200</v>
       </c>
       <c r="M28">
         <v>19327466.25</v>
@@ -1527,7 +1554,7 @@
         <v>320518420.96</v>
       </c>
       <c r="I29">
-        <v>320518420.96</v>
+        <v>944871705.1099999</v>
       </c>
       <c r="J29">
         <v>320518420.96</v>
@@ -1536,7 +1563,7 @@
         <v>944871705.1099999</v>
       </c>
       <c r="L29">
-        <v>944871705.1099999</v>
+        <v>320518420.96</v>
       </c>
       <c r="M29">
         <v>944871705.1099999</v>
@@ -1568,7 +1595,7 @@
         <v>122060612.76</v>
       </c>
       <c r="I30">
-        <v>122060612.76</v>
+        <v>406890966.71999997</v>
       </c>
       <c r="J30">
         <v>122060612.76</v>
@@ -1577,7 +1604,7 @@
         <v>406890966.71999997</v>
       </c>
       <c r="L30">
-        <v>406890966.71999997</v>
+        <v>122060612.76</v>
       </c>
       <c r="M30">
         <v>406890966.71999997</v>
@@ -1609,7 +1636,7 @@
         <v>76856949.2</v>
       </c>
       <c r="I31">
-        <v>76856949.2</v>
+        <v>180862130.62</v>
       </c>
       <c r="J31">
         <v>76856949.2</v>
@@ -1618,7 +1645,7 @@
         <v>180862130.62</v>
       </c>
       <c r="L31">
-        <v>180862130.62</v>
+        <v>76856949.2</v>
       </c>
       <c r="M31">
         <v>180862130.62</v>
@@ -1650,7 +1677,7 @@
         <v>15966222.83</v>
       </c>
       <c r="I32">
-        <v>15966222.83</v>
+        <v>53220742.769999996</v>
       </c>
       <c r="J32">
         <v>15966222.83</v>
@@ -1659,7 +1686,7 @@
         <v>53220742.769999996</v>
       </c>
       <c r="L32">
-        <v>53220742.769999996</v>
+        <v>15966222.83</v>
       </c>
       <c r="M32">
         <v>53220742.769999996</v>
@@ -1691,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>10565030.86</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -1700,7 +1727,7 @@
         <v>10565030.86</v>
       </c>
       <c r="L33">
-        <v>10565030.86</v>
+        <v>0</v>
       </c>
       <c r="M33">
         <v>10565030.86</v>
@@ -1732,7 +1759,7 @@
         <v>54583436.17</v>
       </c>
       <c r="I34">
-        <v>54583436.17</v>
+        <v>181892626.14</v>
       </c>
       <c r="J34">
         <v>54583436.17</v>
@@ -1741,7 +1768,7 @@
         <v>181892626.14</v>
       </c>
       <c r="L34">
-        <v>181892626.14</v>
+        <v>54583436.17</v>
       </c>
       <c r="M34">
         <v>181892626.14</v>
@@ -1773,7 +1800,7 @@
         <v>51051200</v>
       </c>
       <c r="I35">
-        <v>51051200</v>
+        <v>111440208</v>
       </c>
       <c r="J35">
         <v>51051200</v>
@@ -1782,7 +1809,7 @@
         <v>111440208</v>
       </c>
       <c r="L35">
-        <v>111440208</v>
+        <v>51051200</v>
       </c>
       <c r="M35">
         <v>111440208</v>
@@ -1817,13 +1844,13 @@
         <v>50988519.83</v>
       </c>
       <c r="J36">
-        <v>50988518.83</v>
+        <v>50988519.83</v>
       </c>
       <c r="K36">
         <v>50988519.83</v>
       </c>
       <c r="L36">
-        <v>50988519.83</v>
+        <v>50988518.83</v>
       </c>
       <c r="M36">
         <v>50988518.83</v>
@@ -2350,13 +2377,13 @@
         <v>6165819.77</v>
       </c>
       <c r="J49">
-        <v>6165818.77</v>
+        <v>6165819.77</v>
       </c>
       <c r="K49">
         <v>6165819.77</v>
       </c>
       <c r="L49">
-        <v>6165819.77</v>
+        <v>6165818.77</v>
       </c>
       <c r="M49">
         <v>6165818.77</v>
@@ -2552,7 +2579,7 @@
         <v>402167540.94</v>
       </c>
       <c r="I54">
-        <v>402167540.94</v>
+        <v>483216176.94</v>
       </c>
       <c r="J54">
         <v>402167540.94</v>
@@ -2561,7 +2588,7 @@
         <v>483216176.94</v>
       </c>
       <c r="L54">
-        <v>483216176.94</v>
+        <v>402167540.94</v>
       </c>
       <c r="M54">
         <v>483216176.94</v>
@@ -2839,7 +2866,7 @@
         <v>20384540.94</v>
       </c>
       <c r="I61">
-        <v>20384540.94</v>
+        <v>68787976.94</v>
       </c>
       <c r="J61">
         <v>20384540.94</v>
@@ -2848,7 +2875,7 @@
         <v>68787976.94</v>
       </c>
       <c r="L61">
-        <v>68787976.94</v>
+        <v>20384540.94</v>
       </c>
       <c r="M61">
         <v>68787976.94</v>
@@ -3003,7 +3030,7 @@
         <v>2881800</v>
       </c>
       <c r="I65">
-        <v>2881800</v>
+        <v>11947900</v>
       </c>
       <c r="J65">
         <v>2881800</v>
@@ -3012,7 +3039,7 @@
         <v>11947900</v>
       </c>
       <c r="L65">
-        <v>11947900</v>
+        <v>2881800</v>
       </c>
       <c r="M65">
         <v>11947900</v>
@@ -3044,7 +3071,7 @@
         <v>6901200</v>
       </c>
       <c r="I66">
-        <v>6901200</v>
+        <v>30480300</v>
       </c>
       <c r="J66">
         <v>6901200</v>
@@ -3053,7 +3080,7 @@
         <v>30480300</v>
       </c>
       <c r="L66">
-        <v>30480300</v>
+        <v>6901200</v>
       </c>
       <c r="M66">
         <v>30480300</v>
@@ -3372,16 +3399,16 @@
         <v>9776003.81</v>
       </c>
       <c r="I74">
+        <v>138423418.29000002</v>
+      </c>
+      <c r="J74">
         <v>7931090</v>
       </c>
-      <c r="J74">
+      <c r="K74">
+        <v>146681263.10000002</v>
+      </c>
+      <c r="L74">
         <v>9776003.81</v>
-      </c>
-      <c r="K74">
-        <v>138423418.29000002</v>
-      </c>
-      <c r="L74">
-        <v>146681263.10000002</v>
       </c>
       <c r="M74">
         <v>130165573.48</v>
@@ -3413,16 +3440,16 @@
         <v>7931090</v>
       </c>
       <c r="I75">
-        <v>7931090</v>
+        <v>68350214.81</v>
       </c>
       <c r="J75">
         <v>7931090</v>
       </c>
       <c r="K75">
-        <v>68350214.81</v>
+        <v>76608059.62</v>
       </c>
       <c r="L75">
-        <v>76608059.62</v>
+        <v>7931090</v>
       </c>
       <c r="M75">
         <v>60092370</v>
@@ -3454,16 +3481,16 @@
         <v>7931090</v>
       </c>
       <c r="I76">
-        <v>7931090</v>
+        <v>68350214.81</v>
       </c>
       <c r="J76">
         <v>7931090</v>
       </c>
       <c r="K76">
-        <v>68350214.81</v>
+        <v>76608059.62</v>
       </c>
       <c r="L76">
-        <v>76608059.62</v>
+        <v>7931090</v>
       </c>
       <c r="M76">
         <v>60092370</v>
@@ -3618,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <v>0</v>
+        <v>52537600</v>
       </c>
       <c r="J80">
         <v>0</v>
@@ -3627,7 +3654,7 @@
         <v>52537600</v>
       </c>
       <c r="L80">
-        <v>52537600</v>
+        <v>0</v>
       </c>
       <c r="M80">
         <v>52537600</v>
@@ -3659,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="I81">
-        <v>0</v>
+        <v>672600</v>
       </c>
       <c r="J81">
         <v>0</v>
@@ -3668,7 +3695,7 @@
         <v>672600</v>
       </c>
       <c r="L81">
-        <v>672600</v>
+        <v>0</v>
       </c>
       <c r="M81">
         <v>672600</v>
@@ -3700,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="I82">
-        <v>0</v>
+        <v>51865000</v>
       </c>
       <c r="J82">
         <v>0</v>
@@ -3709,7 +3736,7 @@
         <v>51865000</v>
       </c>
       <c r="L82">
-        <v>51865000</v>
+        <v>0</v>
       </c>
       <c r="M82">
         <v>51865000</v>
@@ -3823,10 +3850,10 @@
         <v>10000</v>
       </c>
       <c r="I85">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J85">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="K85">
         <v>10000</v>
@@ -4028,10 +4055,10 @@
         <v>10000</v>
       </c>
       <c r="I90">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J90">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="K90">
         <v>10000</v>
@@ -4274,16 +4301,16 @@
         <v>1834913.81</v>
       </c>
       <c r="I96">
-        <v>0</v>
+        <v>17525603.48</v>
       </c>
       <c r="J96">
-        <v>1834913.81</v>
+        <v>0</v>
       </c>
       <c r="K96">
         <v>17525603.48</v>
       </c>
       <c r="L96">
-        <v>17525603.48</v>
+        <v>1834913.81</v>
       </c>
       <c r="M96">
         <v>17525603.48</v>
@@ -4315,16 +4342,16 @@
         <v>1834913.81</v>
       </c>
       <c r="I97">
-        <v>0</v>
+        <v>3380603.4800000004</v>
       </c>
       <c r="J97">
-        <v>1834913.81</v>
+        <v>0</v>
       </c>
       <c r="K97">
         <v>3380603.4800000004</v>
       </c>
       <c r="L97">
-        <v>3380603.4800000004</v>
+        <v>1834913.81</v>
       </c>
       <c r="M97">
         <v>3380603.4800000004</v>
@@ -4397,7 +4424,7 @@
         <v>0</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>14145000</v>
       </c>
       <c r="J99">
         <v>0</v>
@@ -4406,7 +4433,7 @@
         <v>14145000</v>
       </c>
       <c r="L99">
-        <v>14145000</v>
+        <v>0</v>
       </c>
       <c r="M99">
         <v>14145000</v>
@@ -4725,16 +4752,16 @@
         <v>81240110.53999999</v>
       </c>
       <c r="I107">
+        <v>170241781.28000003</v>
+      </c>
+      <c r="J107">
         <v>80178524.33</v>
       </c>
-      <c r="J107">
+      <c r="K107">
+        <v>171523408.87</v>
+      </c>
+      <c r="L107">
         <v>81740110.53999999</v>
-      </c>
-      <c r="K107">
-        <v>170241781.28000003</v>
-      </c>
-      <c r="L107">
-        <v>171523408.87</v>
       </c>
       <c r="M107">
         <v>169460153.69</v>
@@ -5586,7 +5613,7 @@
         <v>4800000</v>
       </c>
       <c r="I128">
-        <v>4800000</v>
+        <v>12152000</v>
       </c>
       <c r="J128">
         <v>4800000</v>
@@ -5595,7 +5622,7 @@
         <v>12152000</v>
       </c>
       <c r="L128">
-        <v>12152000</v>
+        <v>4800000</v>
       </c>
       <c r="M128">
         <v>12152000</v>
@@ -5668,7 +5695,7 @@
         <v>4800000</v>
       </c>
       <c r="I130">
-        <v>4800000</v>
+        <v>12152000</v>
       </c>
       <c r="J130">
         <v>4800000</v>
@@ -5677,7 +5704,7 @@
         <v>12152000</v>
       </c>
       <c r="L130">
-        <v>12152000</v>
+        <v>4800000</v>
       </c>
       <c r="M130">
         <v>12152000</v>
@@ -5709,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="I131">
-        <v>0</v>
+        <v>56600000</v>
       </c>
       <c r="J131">
         <v>0</v>
@@ -5718,7 +5745,7 @@
         <v>56600000</v>
       </c>
       <c r="L131">
-        <v>56600000</v>
+        <v>0</v>
       </c>
       <c r="M131">
         <v>56600000</v>
@@ -5750,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="I132">
-        <v>0</v>
+        <v>56600000</v>
       </c>
       <c r="J132">
         <v>0</v>
@@ -5759,7 +5786,7 @@
         <v>56600000</v>
       </c>
       <c r="L132">
-        <v>56600000</v>
+        <v>0</v>
       </c>
       <c r="M132">
         <v>56600000</v>
@@ -5996,16 +6023,16 @@
         <v>66431283.3</v>
       </c>
       <c r="I138">
+        <v>91480954.04</v>
+      </c>
+      <c r="J138">
         <v>65369697.09</v>
       </c>
-      <c r="J138">
+      <c r="K138">
+        <v>92762581.63</v>
+      </c>
+      <c r="L138">
         <v>66931283.3</v>
-      </c>
-      <c r="K138">
-        <v>91480954.04</v>
-      </c>
-      <c r="L138">
-        <v>92762581.63</v>
       </c>
       <c r="M138">
         <v>90699326.45</v>
@@ -6037,16 +6064,16 @@
         <v>66431283.3</v>
       </c>
       <c r="I139">
+        <v>91480954.04</v>
+      </c>
+      <c r="J139">
         <v>65369697.09</v>
       </c>
-      <c r="J139">
+      <c r="K139">
+        <v>92762581.63</v>
+      </c>
+      <c r="L139">
         <v>66931283.3</v>
-      </c>
-      <c r="K139">
-        <v>91480954.04</v>
-      </c>
-      <c r="L139">
-        <v>92762581.63</v>
       </c>
       <c r="M139">
         <v>90699326.45</v>
@@ -6734,7 +6761,7 @@
         <v>231473999.96</v>
       </c>
       <c r="I156">
-        <v>231473999.96</v>
+        <v>771546231.13</v>
       </c>
       <c r="J156">
         <v>231473999.96</v>
@@ -6743,7 +6770,7 @@
         <v>771546231.13</v>
       </c>
       <c r="L156">
-        <v>771546231.13</v>
+        <v>231473999.96</v>
       </c>
       <c r="M156">
         <v>771546231.13</v>
@@ -6775,7 +6802,7 @@
         <v>231473999.96</v>
       </c>
       <c r="I157">
-        <v>231473999.96</v>
+        <v>771546231.13</v>
       </c>
       <c r="J157">
         <v>231473999.96</v>
@@ -6784,7 +6811,7 @@
         <v>771546231.13</v>
       </c>
       <c r="L157">
-        <v>771546231.13</v>
+        <v>231473999.96</v>
       </c>
       <c r="M157">
         <v>771546231.13</v>
@@ -6816,7 +6843,7 @@
         <v>134369999.96</v>
       </c>
       <c r="I158">
-        <v>134369999.96</v>
+        <v>439323281.13</v>
       </c>
       <c r="J158">
         <v>134369999.96</v>
@@ -6825,7 +6852,7 @@
         <v>439323281.13</v>
       </c>
       <c r="L158">
-        <v>439323281.13</v>
+        <v>134369999.96</v>
       </c>
       <c r="M158">
         <v>437619281.13</v>
@@ -6857,7 +6884,7 @@
         <v>9120000</v>
       </c>
       <c r="I159">
-        <v>9120000</v>
+        <v>41230000</v>
       </c>
       <c r="J159">
         <v>9120000</v>
@@ -6866,7 +6893,7 @@
         <v>41230000</v>
       </c>
       <c r="L159">
-        <v>41230000</v>
+        <v>9120000</v>
       </c>
       <c r="M159">
         <v>41230000</v>
@@ -6898,7 +6925,7 @@
         <v>24180000</v>
       </c>
       <c r="I160">
-        <v>24180000</v>
+        <v>109313750</v>
       </c>
       <c r="J160">
         <v>24180000</v>
@@ -6907,7 +6934,7 @@
         <v>109313750</v>
       </c>
       <c r="L160">
-        <v>109313750</v>
+        <v>24180000</v>
       </c>
       <c r="M160">
         <v>109313750</v>
@@ -6939,7 +6966,7 @@
         <v>8512000</v>
       </c>
       <c r="I161">
-        <v>8512000</v>
+        <v>28373333.33</v>
       </c>
       <c r="J161">
         <v>8512000</v>
@@ -6948,7 +6975,7 @@
         <v>28373333.33</v>
       </c>
       <c r="L161">
-        <v>28373333.33</v>
+        <v>8512000</v>
       </c>
       <c r="M161">
         <v>28373333.33</v>
@@ -6980,7 +7007,7 @@
         <v>2736000</v>
       </c>
       <c r="I162">
-        <v>2736000</v>
+        <v>11609000</v>
       </c>
       <c r="J162">
         <v>2736000</v>
@@ -6989,7 +7016,7 @@
         <v>11609000</v>
       </c>
       <c r="L162">
-        <v>11609000</v>
+        <v>2736000</v>
       </c>
       <c r="M162">
         <v>11609000</v>
@@ -7062,7 +7089,7 @@
         <v>12000000</v>
       </c>
       <c r="I164">
-        <v>12000000</v>
+        <v>34240650</v>
       </c>
       <c r="J164">
         <v>12000000</v>
@@ -7071,7 +7098,7 @@
         <v>34240650</v>
       </c>
       <c r="L164">
-        <v>34240650</v>
+        <v>12000000</v>
       </c>
       <c r="M164">
         <v>30136650</v>
@@ -7103,7 +7130,7 @@
         <v>22567999.96</v>
       </c>
       <c r="I165">
-        <v>22567999.96</v>
+        <v>75226666.55000001</v>
       </c>
       <c r="J165">
         <v>22567999.96</v>
@@ -7112,7 +7139,7 @@
         <v>75226666.55000001</v>
       </c>
       <c r="L165">
-        <v>75226666.55000001</v>
+        <v>22567999.96</v>
       </c>
       <c r="M165">
         <v>75226666.55000001</v>
@@ -7144,7 +7171,7 @@
         <v>7254000</v>
       </c>
       <c r="I166">
-        <v>7254000</v>
+        <v>30779125</v>
       </c>
       <c r="J166">
         <v>7254000</v>
@@ -7153,7 +7180,7 @@
         <v>30779125</v>
       </c>
       <c r="L166">
-        <v>30779125</v>
+        <v>7254000</v>
       </c>
       <c r="M166">
         <v>30779125</v>
@@ -7226,7 +7253,7 @@
         <v>48000000</v>
       </c>
       <c r="I168">
-        <v>48000000</v>
+        <v>108550756.25</v>
       </c>
       <c r="J168">
         <v>48000000</v>
@@ -7235,7 +7262,7 @@
         <v>108550756.25</v>
       </c>
       <c r="L168">
-        <v>108550756.25</v>
+        <v>48000000</v>
       </c>
       <c r="M168">
         <v>110950756.25</v>
@@ -7267,7 +7294,7 @@
         <v>97104000</v>
       </c>
       <c r="I169">
-        <v>97104000</v>
+        <v>332222950</v>
       </c>
       <c r="J169">
         <v>97104000</v>
@@ -7276,7 +7303,7 @@
         <v>332222950</v>
       </c>
       <c r="L169">
-        <v>332222950</v>
+        <v>97104000</v>
       </c>
       <c r="M169">
         <v>333926950</v>
@@ -7308,7 +7335,7 @@
         <v>27360000</v>
       </c>
       <c r="I170">
-        <v>27360000</v>
+        <v>132418125</v>
       </c>
       <c r="J170">
         <v>27360000</v>
@@ -7317,7 +7344,7 @@
         <v>132418125</v>
       </c>
       <c r="L170">
-        <v>132418125</v>
+        <v>27360000</v>
       </c>
       <c r="M170">
         <v>132418125</v>
@@ -7349,7 +7376,7 @@
         <v>25536000</v>
       </c>
       <c r="I171">
-        <v>25536000</v>
+        <v>85120000</v>
       </c>
       <c r="J171">
         <v>25536000</v>
@@ -7358,7 +7385,7 @@
         <v>85120000</v>
       </c>
       <c r="L171">
-        <v>85120000</v>
+        <v>25536000</v>
       </c>
       <c r="M171">
         <v>85120000</v>
@@ -7390,7 +7417,7 @@
         <v>8208000</v>
       </c>
       <c r="I172">
-        <v>8208000</v>
+        <v>32148000</v>
       </c>
       <c r="J172">
         <v>8208000</v>
@@ -7399,7 +7426,7 @@
         <v>32148000</v>
       </c>
       <c r="L172">
-        <v>32148000</v>
+        <v>8208000</v>
       </c>
       <c r="M172">
         <v>35397000</v>
@@ -7431,7 +7458,7 @@
         <v>36000000</v>
       </c>
       <c r="I173">
-        <v>36000000</v>
+        <v>82536825</v>
       </c>
       <c r="J173">
         <v>36000000</v>
@@ -7440,7 +7467,7 @@
         <v>82536825</v>
       </c>
       <c r="L173">
-        <v>82536825</v>
+        <v>36000000</v>
       </c>
       <c r="M173">
         <v>80991825</v>
@@ -7513,7 +7540,7 @@
         <v>8560843.35</v>
       </c>
       <c r="I175">
-        <v>8560843.35</v>
+        <v>33260843.35</v>
       </c>
       <c r="J175">
         <v>8560843.35</v>
@@ -7522,7 +7549,7 @@
         <v>33260843.35</v>
       </c>
       <c r="L175">
-        <v>33260843.35</v>
+        <v>8560843.35</v>
       </c>
       <c r="M175">
         <v>33260843.35</v>
@@ -7554,7 +7581,7 @@
         <v>8560843.35</v>
       </c>
       <c r="I176">
-        <v>8560843.35</v>
+        <v>33260843.35</v>
       </c>
       <c r="J176">
         <v>8560843.35</v>
@@ -7563,7 +7590,7 @@
         <v>33260843.35</v>
       </c>
       <c r="L176">
-        <v>33260843.35</v>
+        <v>8560843.35</v>
       </c>
       <c r="M176">
         <v>33260843.35</v>
@@ -7636,7 +7663,7 @@
         <v>0</v>
       </c>
       <c r="I178">
-        <v>0</v>
+        <v>24700000</v>
       </c>
       <c r="J178">
         <v>0</v>
@@ -7645,7 +7672,7 @@
         <v>24700000</v>
       </c>
       <c r="L178">
-        <v>24700000</v>
+        <v>0</v>
       </c>
       <c r="M178">
         <v>24700000</v>

</xml_diff>